<commit_message>
🔄 Actualización automática del tracker
</commit_message>
<xml_diff>
--- a/tracker_resultados.xlsx
+++ b/tracker_resultados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,10 +504,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>-1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -538,10 +540,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>-1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -572,14 +576,16 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>14266295</v>
+        <v>14266950</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -588,32 +594,34 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Anna Kalinskaya</t>
+          <t>Nishesh Basavareddy</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Elina Svitolina</t>
+          <t>Zachary Svajda</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Gana Anna Kalinskaya</t>
+          <t>Gana Zachary Svajda</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>3.2</v>
+        <v>5.5</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>14266898</v>
+        <v>14266954</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -622,32 +630,34 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Elias Ymer</t>
+          <t>Michael Zheng</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Hugo Grenier</t>
+          <t>Yu Hsiou Hsu</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Gana Elias Ymer</t>
+          <t>Gana Yu Hsiou Hsu</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>23</v>
+        <v>2.38</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>1.38</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>14266950</v>
+        <v>14267299</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -656,32 +666,34 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Nishesh Basavareddy</t>
+          <t>Daniel Michalski</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Zachary Svajda</t>
+          <t>Valentin Vacherot</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Gana Zachary Svajda</t>
+          <t>Gana Daniel Michalski</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>14266954</v>
+        <v>14266295</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -690,100 +702,94 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Michael Zheng</t>
+          <t>Anna Kalinskaya</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Yu Hsiou Hsu</t>
+          <t>Elina Svitolina</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Gana Yu Hsiou Hsu</t>
+          <t>Gana Anna Kalinskaya</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>2.38</v>
+        <v>3.4</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>-1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>14267299</v>
+        <v>14259084</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-08-01</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Daniel Michalski</t>
+          <t>Abdullah Shelbayh</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Valentin Vacherot</t>
+          <t>Alexandr Binda</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Gana Daniel Michalski</t>
+          <t>Gana Alexandr Binda</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>3</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>3.25</v>
+      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>14266295</v>
+        <v>14266653</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-08-01</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Anna Kalinskaya</t>
+          <t>Botic Van de Zandschulp</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Elina Svitolina</t>
+          <t>Guy Den Ouden</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Gana Anna Kalinskaya</t>
+          <t>Gana Guy Den Ouden</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>3.25</v>
+      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>14259084</v>
+        <v>14266660</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -792,32 +798,28 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Abdullah Shelbayh</t>
+          <t>Olle Wallin</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Alexandr Binda</t>
+          <t>Vilius Gaubas</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Gana Alexandr Binda</t>
+          <t>Gana Olle Wallin</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>4.5</v>
+      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>14266653</v>
+        <v>14265591</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -826,62 +828,24 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Botic Van de Zandschulp</t>
+          <t>Alexei Popyrin</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Guy Den Ouden</t>
+          <t>Holger Rune</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Gana Guy Den Ouden</t>
+          <t>Gana Holger Rune</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+        <v>1.4</v>
+      </c>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>14266660</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2025-08-02</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Olle Wallin</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Vilius Gaubas</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Gana Olle Wallin</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker (cada 3h)
</commit_message>
<xml_diff>
--- a/tracker_resultados.xlsx
+++ b/tracker_resultados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1195,6 +1195,390 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>14339214</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2025-08-04</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Clement Chidekh</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Harold Mayot</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Gana Clement Chidekh</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>14339495</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2025-08-04</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Carlos Taberner</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Federico Bondioli</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Gana Federico Bondioli</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>5</v>
+      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>14339492</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2025-08-04</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Gabriele Piraino</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Jelle Sels</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Gana Jelle Sels</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>14339490</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2025-08-04</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Kimmer Coppejans</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Tiago Pereira</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Gana Tiago Pereira</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>14339485</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2025-08-04</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Murkel Dellien</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Dusan Lajovic</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Gana Murkel Dellien</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>14339491</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2025-08-04</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Oleg Prihodko</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Stefano Travaglia</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Gana Oleg Prihodko</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>14339487</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2025-08-04</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Santiago Rodriguez Taverna</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Nikolas Sanchez Izquierdo</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Gana Santiago Rodriguez Taverna</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>14339504</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2025-08-04</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Benjamin Hassan</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Filip Cristian Jianu</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Gana Filip Cristian Jianu</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>14339502</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2025-08-04</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Jan Choinski</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Geoffrey Blancaneaux</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Gana Geoffrey Blancaneaux</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>14339501</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2025-08-04</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Joao Lucas Reis Da Silva</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Olle Wallin</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Gana Olle Wallin</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>14339505</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2025-08-04</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Joel Schwaerzler</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Christoph Negritu</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Gana Christoph Negritu</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>14339509</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2025-08-04</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Vilius Gaubas</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Diego Dedura-Palomero</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Gana Diego Dedura-Palomero</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>